<commit_message>
DB & BE noisy space feature for subject
</commit_message>
<xml_diff>
--- a/templates/subject_template.xlsx
+++ b/templates/subject_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitHubRepos_4\Siba23k\Siba_be\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\siba-be\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820104D9-315E-4A98-AB99-707551935D80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D50672F-5C11-49E5-B7BF-57C10A6DC23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{41C36109-A372-6C4A-A6DF-311FC9062FC4}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{41C36109-A372-6C4A-A6DF-311FC9062FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Name of the lesson</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Esitystila</t>
+  </si>
+  <si>
+    <t>isNoisy</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -141,9 +147,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +187,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -287,7 +293,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,7 +435,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,25 +443,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59273CB-FF1A-B844-9868-D9A40C06FA28}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
     <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +486,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -506,8 +515,11 @@
       <c r="H2" t="s">
         <v>9</v>
       </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -532,8 +544,11 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -557,6 +572,9 @@
       </c>
       <c r="H4" t="s">
         <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>